<commit_message>
Add new row to Card7
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -3771,7 +3771,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3843,7 +3843,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -3851,9 +3851,7 @@
       <c r="C2" t="n">
         <v>150</v>
       </c>
-      <c r="D2" t="n">
-        <v>60</v>
-      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -4066,6 +4064,48 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>1\9\2025</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'other' to Card7
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -3771,7 +3771,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3840,6 +3840,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -3860,6 +3865,7 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -3884,6 +3890,7 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -3904,6 +3911,7 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -3924,6 +3932,7 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -3944,6 +3953,7 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -3964,6 +3974,7 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -3984,6 +3995,7 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -4004,6 +4016,7 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -4024,6 +4037,7 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -4044,6 +4058,7 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -4064,48 +4079,7 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>done</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>done</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>1\9\2025</t>
-        </is>
-      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Event' to Card18
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -5496,7 +5496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5577,242 +5577,94 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>done</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1\2\2024</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>تم تشغيل ماكينه</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>م/محمد عبدالله</t>
-        </is>
-      </c>
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>150</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>151</v>
+      </c>
+      <c r="C3" t="n">
+        <v>300</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>  </t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>21\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>301</v>
+      </c>
+      <c r="C4" t="n">
+        <v>450</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>451</v>
+      </c>
+      <c r="C5" t="n">
+        <v>550</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5828,165 +5680,77 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>19\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>573.0</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>551</v>
+      </c>
+      <c r="C6" t="n">
+        <v>700</v>
+      </c>
+      <c r="D6" t="n">
+        <v>573</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>8\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>729.0</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>701</v>
+      </c>
+      <c r="C7" t="n">
+        <v>850</v>
+      </c>
+      <c r="D7" t="n">
+        <v>729</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5997,43 +5761,23 @@
           <t>7\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>869.0</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>851</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>869</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6044,401 +5788,105 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>30\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1150</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1151</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1301</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1450</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1451</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9813,7 +9261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9882,6 +9330,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -9908,6 +9361,7 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -9940,6 +9394,7 @@
           <t>1\12\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -9960,6 +9415,7 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -9992,6 +9448,7 @@
           <t>11\3\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -10026,6 +9483,7 @@
           <t>29\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -10056,6 +9514,7 @@
           <t>20\8\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -10090,6 +9549,7 @@
           <t>23\10\2025</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -10110,6 +9570,7 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -10130,6 +9591,7 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -10150,6 +9612,7 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -10170,6 +9633,7 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Correction' to Card18
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -9261,7 +9261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9335,6 +9335,11 @@
           <t>event</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -9397,7 +9402,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -9460,7 +9470,12 @@
           <t>1\12\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -9523,7 +9538,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -9586,7 +9606,12 @@
           <t>11\3\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -9649,7 +9674,12 @@
           <t>29\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -9712,7 +9742,12 @@
           <t>20\8\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -9775,7 +9810,12 @@
           <t>23\10\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -9838,7 +9878,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -9901,7 +9946,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -9964,7 +10014,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -10027,7 +10082,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new row to Card18
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -9261,7 +9261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9357,8 +9357,16 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>nan</t>
@@ -10122,6 +10130,46 @@
       <c r="N12" t="inlineStr">
         <is>
           <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>13\8\2025</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Dfk belt  947*2.5*1.5 قطع سير</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>تم تغير سير+تم تشحيم الماكينه بالكامل</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new column 'Servised by' to Card18
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -9261,7 +9261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9340,6 +9340,11 @@
           <t>Correction</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Servised by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -9412,6 +9417,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -9484,6 +9490,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -9556,6 +9563,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -9628,6 +9636,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -9700,6 +9709,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -9772,6 +9782,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -9844,6 +9855,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -9916,6 +9928,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -9988,6 +10001,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -10060,6 +10074,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -10132,6 +10147,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -10204,6 +10220,7 @@
           <t>تم تغير سير+تم تشحيم الماكينه بالكامل</t>
         </is>
       </c>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new row under range 151-300 in Card18
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -9261,7 +9261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10267,6 +10267,39 @@
       <c r="O13" t="inlineStr">
         <is>
           <t>حسام السيد</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>محمد عبدالله</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new row under range 301-450 in Card18
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -9261,7 +9261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9585,72 +9585,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>11\3\2025</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>محمد عبدالله</t>
         </is>
       </c>
     </row>
@@ -9662,17 +9618,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>550</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>590</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -9682,22 +9638,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -9712,7 +9668,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>29\4\2025</t>
+          <t>11\3\2025</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -9739,17 +9695,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>700</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>785</t>
+          <t>590</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -9759,7 +9715,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -9769,12 +9725,12 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -9789,7 +9745,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>20\8\2025</t>
+          <t>29\4\2025</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -9816,17 +9772,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>850</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>883</t>
+          <t>785</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -9841,7 +9797,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -9866,7 +9822,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>23\10\2025</t>
+          <t>20\8\2025</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -9893,17 +9849,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>883</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -9913,12 +9869,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -9943,7 +9899,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>23\10\2025</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -9970,12 +9926,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>1150</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -10047,12 +10003,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1301</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1450</t>
+          <t>1300</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -10124,12 +10080,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1451</t>
+          <t>1301</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>1450</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -10201,12 +10157,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>1451</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -10251,22 +10207,22 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>13\8\2024</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Dfk belt  947*2.5*1.5 قطع سير</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>تم تغير سير+تم تشحيم الماكينه بالكامل</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>حسام السيد</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -10286,18 +10242,139 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>13\8\2024</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Dfk belt  947*2.5*1.5 قطع سير</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>تم تغير سير+تم تشحيم الماكينه بالكامل</t>
+        </is>
+      </c>
       <c r="O14" t="inlineStr">
+        <is>
+          <t>حسام السيد</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
         <is>
           <t>محمد عبدالله</t>
         </is>

</xml_diff>

<commit_message>
Delete rows [3, 12, 13] from Card18
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -9261,7 +9261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9585,12 +9585,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>550</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -9605,12 +9605,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -9635,7 +9635,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>11\3\2025</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -9650,7 +9650,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>محمد عبدالله</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -9662,17 +9662,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>700</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>590</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -9682,22 +9682,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -9712,7 +9712,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>11\3\2025</t>
+          <t>29\4\2025</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -9739,17 +9739,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>850</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>590</t>
+          <t>785</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -9759,7 +9759,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -9769,12 +9769,12 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -9789,7 +9789,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>29\4\2025</t>
+          <t>20\8\2025</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -9816,17 +9816,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>785</t>
+          <t>883</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -9841,7 +9841,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -9866,7 +9866,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>20\8\2025</t>
+          <t>23\10\2025</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -9893,17 +9893,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1150</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>883</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -9913,12 +9913,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -9943,7 +9943,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>23\10\2025</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -9970,12 +9970,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>1300</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -10047,12 +10047,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>1301</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>1450</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -10124,12 +10124,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1301</t>
+          <t>1451</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1450</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -10190,237 +10190,6 @@
       <c r="O12" t="inlineStr">
         <is>
           <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>محمد عبدالله</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new row under range 151-301 in Card24
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,7 +585,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -595,54 +595,26 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>301</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>222</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>  </t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -652,12 +624,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -682,7 +654,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>  </t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -714,12 +686,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>450</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -776,17 +748,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>550</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>632</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -796,22 +768,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -826,7 +798,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>20\5\2025</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -838,17 +810,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>700</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>870</t>
+          <t>632</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -868,27 +840,27 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>6\10\2025</t>
+          <t>20\5\2025</t>
         </is>
       </c>
     </row>
@@ -900,57 +872,57 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>850</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>870</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>6\10\2025</t>
         </is>
       </c>
     </row>
@@ -962,12 +934,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1024,12 +996,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>1150</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1086,12 +1058,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1301</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1450</t>
+          <t>1300</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1148,12 +1120,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1451</t>
+          <t>1301</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>1450</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1205,40 +1177,126 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>24</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>151</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>300</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>222</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>done</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>done</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Delete rows [1, 2] from Card24
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,7 +585,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -595,17 +595,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -620,7 +620,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>  </t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -647,36 +647,64 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>450</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>222</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>done</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -686,12 +714,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>550</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -716,7 +744,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>  </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -748,57 +776,57 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>700</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>632</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>20\5\2025</t>
         </is>
       </c>
     </row>
@@ -810,57 +838,57 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>850</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>870</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>6\10\2025</t>
         </is>
       </c>
     </row>
@@ -872,17 +900,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>632</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -892,22 +920,22 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -922,7 +950,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>20\5\2025</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -934,17 +962,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>1150</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>870</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -954,12 +982,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -984,7 +1012,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>6\10\2025</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -996,12 +1024,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1300</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1058,12 +1086,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>1301</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>1450</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1120,12 +1148,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>1451</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1177,184 +1205,60 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1301</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1450</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>222</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>222</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>done</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>done</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
         <is>
           <t>nan</t>
         </is>

</xml_diff>

<commit_message>
Edit sheet Card23 by HOSSAM
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -536,51 +536,15 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -598,51 +562,19 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>  </t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -660,51 +592,15 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -722,51 +618,15 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -789,11 +649,7 @@
           <t>632</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -814,16 +670,8 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\5\2025</t>
@@ -851,11 +699,7 @@
           <t>870</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -866,26 +710,10 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>6\10\2025</t>
@@ -908,51 +736,15 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -970,51 +762,15 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1032,51 +788,15 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1094,51 +814,15 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1156,51 +840,15 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1233,36 +881,12 @@
           <t>done</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5008,36 +4632,88 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5048,15 +4724,31 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>  </t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>6\8\2024</t>
@@ -5064,36 +4756,88 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5109,14 +4853,26 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>23\1\2025</t>
@@ -5124,29 +4880,61 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>641</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>641</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>15\5\2025</t>
@@ -5154,19 +4942,31 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>836</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>836</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5177,10 +4977,26 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>4\9\2025</t>
@@ -5188,104 +5004,314 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Correction ' to Card1 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7205,7 +7205,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7279,6 +7279,11 @@
           <t>Event</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Correction </t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -7341,7 +7346,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7404,7 +7414,12 @@
           <t>15\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7467,7 +7482,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7530,7 +7550,12 @@
           <t>29\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7593,7 +7618,12 @@
           <t>5\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7656,7 +7686,12 @@
           <t>5\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7719,7 +7754,12 @@
           <t>24\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -7782,7 +7822,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7845,7 +7890,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -7908,7 +7958,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -7971,7 +8026,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Serviced by ' to Card1 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7205,7 +7205,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7281,7 +7281,12 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Correction </t>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serviced by </t>
         </is>
       </c>
     </row>
@@ -7351,7 +7356,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7419,7 +7429,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7487,7 +7502,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7555,7 +7575,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7623,7 +7648,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7691,7 +7721,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7759,7 +7794,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -7827,7 +7867,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7895,7 +7940,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -7963,7 +8013,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8031,7 +8086,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Crrection' to Card1 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7205,7 +7205,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7289,6 +7289,11 @@
           <t>Serviced by</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Crrection</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -7351,7 +7356,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N2" t="inlineStr">
         <is>
           <t>nan</t>
@@ -7362,6 +7371,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7424,7 +7434,11 @@
           <t>15\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N3" t="inlineStr">
         <is>
           <t>nan</t>
@@ -7435,6 +7449,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7497,7 +7512,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N4" t="inlineStr">
         <is>
           <t>nan</t>
@@ -7508,6 +7527,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7570,7 +7590,11 @@
           <t>29\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N5" t="inlineStr">
         <is>
           <t>nan</t>
@@ -7581,6 +7605,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7643,7 +7668,11 @@
           <t>5\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N6" t="inlineStr">
         <is>
           <t>nan</t>
@@ -7654,6 +7683,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7716,7 +7746,11 @@
           <t>5\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N7" t="inlineStr">
         <is>
           <t>nan</t>
@@ -7727,6 +7761,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7789,7 +7824,11 @@
           <t>24\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N8" t="inlineStr">
         <is>
           <t>nan</t>
@@ -7800,6 +7839,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -7862,7 +7902,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N9" t="inlineStr">
         <is>
           <t>nan</t>
@@ -7873,6 +7917,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7935,7 +7980,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N10" t="inlineStr">
         <is>
           <t>nan</t>
@@ -7946,6 +7995,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8008,7 +8058,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N11" t="inlineStr">
         <is>
           <t>nan</t>
@@ -8019,6 +8073,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8081,7 +8136,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N12" t="inlineStr">
         <is>
           <t>nan</t>
@@ -8092,6 +8151,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new row under range 0-150 in Card1 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7205,7 +7205,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7371,7 +7371,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7381,72 +7385,40 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>150</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>159</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>  </t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>15\7\2024</t>
-        </is>
-      </c>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>تم تركيب وعيار ماكينه</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">تم التشغيل </t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>م.الشناوي</t>
         </is>
       </c>
       <c r="P3" t="inlineStr"/>
@@ -7459,27 +7431,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>159</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -7489,7 +7461,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>  </t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -7509,7 +7481,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>15\7\2024</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -7527,7 +7499,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7537,12 +7513,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>450</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -7552,17 +7528,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -7572,7 +7548,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -7587,7 +7563,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>29\1\2025</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -7605,7 +7581,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr"/>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7615,47 +7595,47 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>550</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>565</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -7665,7 +7645,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>5\4\2025</t>
+          <t>29\1\2025</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -7683,7 +7663,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7693,17 +7677,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>700</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>724</t>
+          <t>565</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -7713,7 +7697,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -7723,7 +7707,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -7733,17 +7717,17 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>5\7\2025</t>
+          <t>5\4\2025</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -7761,7 +7745,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr"/>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7771,17 +7759,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>850</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>859</t>
+          <t>724</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -7791,12 +7779,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -7816,12 +7804,12 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>24\9\2025</t>
+          <t>5\7\2025</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -7839,7 +7827,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -7849,17 +7841,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>859</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -7874,7 +7866,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -7899,7 +7891,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>24\9\2025</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -7917,7 +7909,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr"/>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7927,12 +7923,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>1150</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -7995,7 +7991,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr"/>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8005,12 +8005,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1301</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1450</t>
+          <t>1300</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -8073,7 +8073,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr"/>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8083,75 +8087,161 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>1451</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Edit sheet Card1 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7398,14 +7398,46 @@
           <t>.1</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="M3" t="inlineStr">
         <is>
           <t>تم تركيب وعيار ماكينه</t>
@@ -7421,7 +7453,11 @@
           <t>م.الشناوي</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">

</xml_diff>

<commit_message>
Delete rows [1] from Card1 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7205,7 +7205,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7385,27 +7385,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>.1</t>
+          <t>159</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -7415,7 +7415,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>  </t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -7435,22 +7435,22 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>15\7\2024</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>تم تركيب وعيار ماكينه</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t xml:space="preserve">تم التشغيل </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>م.الشناوي</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -7467,27 +7467,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>450</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>159</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -7497,7 +7497,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>  </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -7517,7 +7517,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>15\7\2024</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -7549,12 +7549,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>550</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -7564,17 +7564,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -7599,7 +7599,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>29\1\2025</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -7631,47 +7631,47 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>700</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>565</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -7681,7 +7681,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>29\1\2025</t>
+          <t>5\4\2025</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -7713,17 +7713,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>850</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>565</t>
+          <t>724</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -7733,7 +7733,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -7743,7 +7743,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -7753,17 +7753,17 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>5\4\2025</t>
+          <t>5\7\2025</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -7795,17 +7795,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>724</t>
+          <t>859</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -7815,12 +7815,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -7840,12 +7840,12 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>5\7\2025</t>
+          <t>24\9\2025</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -7877,17 +7877,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1150</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>859</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -7902,7 +7902,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -7927,7 +7927,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>24\9\2025</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -7959,12 +7959,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>1300</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -8041,12 +8041,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>1301</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>1450</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -8123,12 +8123,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1301</t>
+          <t>1451</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1450</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -8192,88 +8192,6 @@
         </is>
       </c>
       <c r="P12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>

</xml_diff>

<commit_message>
Add new column 'Correction' to Card1 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7037,7 +7037,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7116,6 +7116,11 @@
           <t>Event</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -7183,7 +7188,12 @@
           <t xml:space="preserve"> محمد عبدالله</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7251,7 +7261,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7319,7 +7334,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7387,7 +7407,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7455,7 +7480,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7523,7 +7553,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7591,7 +7626,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -7659,7 +7699,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7727,7 +7772,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -7795,7 +7845,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -7863,7 +7918,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Event ' to Card23 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -4479,7 +4479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4548,38 +4548,96 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Event </t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4590,48 +4648,122 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>6\8\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4647,64 +4779,122 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>23\1\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>641</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>641</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>15\5\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>836</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>836</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4715,115 +4905,347 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>4\9\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7143,41 +7565,13 @@
           <t>1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
           <t>1\2\2024</t>
@@ -7188,16 +7582,8 @@
           <t xml:space="preserve"> محمد عبدالله</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7230,51 +7616,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>15\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7292,66 +7646,18 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7369,11 +7675,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7389,46 +7691,22 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>29\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7451,61 +7729,29 @@
           <t>565</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>5\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7528,36 +7774,16 @@
           <t>724</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7568,21 +7794,9 @@
           <t>5\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7605,61 +7819,25 @@
           <t>859</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>24\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -7677,66 +7855,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7754,66 +7884,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -7831,66 +7913,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -7908,66 +7942,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Correction ' to Card23 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -4479,7 +4479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4550,7 +4550,12 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Event </t>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Correction </t>
         </is>
       </c>
     </row>
@@ -4615,7 +4620,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4678,7 +4688,12 @@
           <t>6\8\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4741,7 +4756,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4804,7 +4824,12 @@
           <t>23\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4867,7 +4892,12 @@
           <t>15\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -4930,7 +4960,12 @@
           <t>4\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -4993,7 +5028,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -5056,7 +5096,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -5119,7 +5164,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -5182,7 +5232,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -5245,7 +5300,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Serviced by ' to Card23 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -4479,7 +4479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4555,7 +4555,12 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Correction </t>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serviced by </t>
         </is>
       </c>
     </row>
@@ -4625,7 +4630,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4693,7 +4703,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4761,7 +4776,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4829,7 +4849,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4897,7 +4922,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -4965,7 +4995,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -5033,7 +5068,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -5101,7 +5141,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -5169,7 +5214,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -5237,7 +5287,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -5305,7 +5360,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Correction' to Card24 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,11 @@
           <t>Event</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -586,7 +591,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -649,7 +659,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -712,7 +727,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -775,7 +795,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -838,7 +863,12 @@
           <t>20\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -901,7 +931,12 @@
           <t>6\10\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -964,7 +999,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1027,7 +1067,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1090,7 +1135,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1153,7 +1203,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1216,7 +1271,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Event' to Card23 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,306 +519,105 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>150</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>151</v>
+      </c>
+      <c r="C3" t="n">
+        <v>300</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>  </t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>301</v>
+      </c>
+      <c r="C4" t="n">
+        <v>450</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>451</v>
+      </c>
+      <c r="C5" t="n">
+        <v>550</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>632</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>551</v>
+      </c>
+      <c r="C6" t="n">
+        <v>700</v>
+      </c>
+      <c r="D6" t="n">
+        <v>632</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -839,53 +638,28 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>870</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>701</v>
+      </c>
+      <c r="C7" t="n">
+        <v>850</v>
+      </c>
+      <c r="D7" t="n">
+        <v>870</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -896,371 +670,115 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>6\10\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>851</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1150</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1151</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1301</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1450</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1451</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4935,7 +4453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5004,38 +4522,96 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5046,52 +4622,122 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>  </t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>6\8\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5107,64 +4753,122 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>23\1\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>641</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>641</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>15\5\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>836</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>836</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5175,115 +4879,347 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>4\9\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Edit sheet Card23 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -4531,7 +4531,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -4589,12 +4589,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -4652,12 +4656,16 @@
           <t>6\8\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -4715,12 +4723,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -4778,12 +4790,16 @@
           <t>23\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -4841,12 +4857,16 @@
           <t>15\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -4904,12 +4924,16 @@
           <t>4\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -4967,12 +4991,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -5030,12 +5058,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -5093,12 +5125,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -5156,12 +5192,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -5219,7 +5259,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Correction' to Card23 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -4535,7 +4535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4609,6 +4609,11 @@
           <t>Event</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4671,7 +4676,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4734,7 +4744,12 @@
           <t>6\8\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4797,7 +4812,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4860,7 +4880,12 @@
           <t>23\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4923,7 +4948,12 @@
           <t>15\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -4986,7 +5016,12 @@
           <t>4\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -5049,7 +5084,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -5112,7 +5152,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -5175,7 +5220,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -5238,7 +5288,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -5301,7 +5356,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Servised by' to Card23 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -4535,7 +4535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4614,6 +4614,11 @@
           <t>Correction</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Servised by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4681,7 +4686,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4749,7 +4759,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4817,7 +4832,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4885,7 +4905,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4953,7 +4978,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5021,7 +5051,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -5089,7 +5124,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -5157,7 +5197,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -5225,7 +5270,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -5293,7 +5343,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -5361,7 +5416,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Event' to Card22 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -4636,46 +4636,14 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
           <t>1\2\2023</t>
@@ -4686,11 +4654,7 @@
           <t>تم التشغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>م.صيام</t>
@@ -4713,11 +4677,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4728,51 +4688,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>6\8\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4790,66 +4718,18 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4867,11 +4747,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4887,46 +4763,22 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>23\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4949,61 +4801,25 @@
           <t>641</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>15\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5026,11 +4842,7 @@
           <t>836</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5041,46 +4853,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>4\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -5098,66 +4882,18 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -5175,66 +4911,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -5252,66 +4940,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -5329,66 +4969,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -5406,66 +4998,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8539,7 +8083,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8608,78 +8152,222 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8695,64 +8383,122 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>25\1\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>629</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>629</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>14\5\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>800</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8763,115 +8509,347 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>1\9\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Correction' to Card22 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -8083,7 +8083,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8157,6 +8157,11 @@
           <t>Event</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -8219,7 +8224,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -8282,7 +8292,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8345,7 +8360,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8408,7 +8428,12 @@
           <t>25\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8471,7 +8496,12 @@
           <t>14\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8534,7 +8564,12 @@
           <t>1\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8597,7 +8632,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -8660,7 +8700,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8723,7 +8768,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8786,7 +8836,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8849,7 +8904,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Servised by' to Card22 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -8083,7 +8083,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8162,6 +8162,11 @@
           <t>Correction</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Servised by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -8229,7 +8234,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -8297,7 +8307,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8365,7 +8380,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8433,7 +8453,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8501,7 +8526,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8569,7 +8599,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8637,7 +8672,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -8705,7 +8745,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8773,7 +8818,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8841,7 +8891,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8909,7 +8964,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Edit sheet Card22 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -8171,7 +8171,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -8239,12 +8239,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -8312,12 +8316,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -8385,12 +8393,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -8458,12 +8470,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -8531,12 +8547,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -8604,12 +8624,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -8677,12 +8701,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -8750,12 +8778,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -8823,12 +8855,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -8896,12 +8932,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -8969,7 +9009,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new row under range 0-150 in Card23 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -4535,7 +4535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4623,7 +4623,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -4636,7 +4636,11 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -4644,22 +4648,10 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1\2\2023</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>تم التشغيل</t>
-        </is>
-      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>م.صيام</t>
-        </is>
-      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4669,38 +4661,74 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>6\8\2024</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+          <t>1\2\2023</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>تم التشغيل</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>م.صيام</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4710,26 +4738,74 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>6\8\2024</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4739,46 +4815,74 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>23\1\2025</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4788,38 +4892,74 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>550</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>641</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>15\5\2025</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+          <t>23\1\2025</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -4829,42 +4969,74 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>700</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>836</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>641</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>4\9\2025</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+          <t>15\5\2025</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -4874,26 +5046,74 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>836</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>4\9\2025</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -4903,26 +5123,74 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -4932,26 +5200,74 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -4961,26 +5277,74 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1301</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -4990,26 +5354,151 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>1451</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8184,61 +8673,21 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
           <t>تم التشغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>ا.نادر</t>
@@ -8261,66 +8710,18 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8338,66 +8739,18 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8415,11 +8768,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8435,46 +8784,22 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>25\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8497,61 +8822,25 @@
           <t>629</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>14\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8574,11 +8863,7 @@
           <t>800</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8589,46 +8874,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>1\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8646,66 +8903,18 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -8723,66 +8932,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8800,66 +8961,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8877,66 +8990,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8954,66 +9019,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Delete rows [0] from Card23 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -4535,7 +4535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4678,12 +4678,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>1\2\2023</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>تم التشغيل</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -4693,7 +4693,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>م.صيام</t>
         </is>
       </c>
     </row>
@@ -4705,27 +4705,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -4755,12 +4755,12 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>1\2\2023</t>
+          <t>6\8\2024</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>تم التشغيل</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -4770,7 +4770,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>م.صيام</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -4782,12 +4782,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>450</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -4797,12 +4797,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -4832,7 +4832,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>6\8\2024</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -4859,12 +4859,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>550</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -4874,17 +4874,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -4894,7 +4894,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -4909,7 +4909,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>23\1\2025</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -4936,42 +4936,42 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>700</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>641</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -4986,7 +4986,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>23\1\2025</t>
+          <t>15\5\2025</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -5013,17 +5013,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>850</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>641</t>
+          <t>836</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -5033,17 +5033,17 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -5063,7 +5063,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>15\5\2025</t>
+          <t>4\9\2025</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -5090,17 +5090,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>836</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -5110,12 +5110,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -5140,7 +5140,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>4\9\2025</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -5167,12 +5167,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1150</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -5244,12 +5244,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>1300</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -5321,12 +5321,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>1301</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>1450</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -5398,12 +5398,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1301</t>
+          <t>1451</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1450</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -5462,83 +5462,6 @@
         </is>
       </c>
       <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>

</xml_diff>

<commit_message>
Edit sheet Card3 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -4641,41 +4641,13 @@
           <t>1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
           <t>1\2\2023</t>
@@ -4686,11 +4658,7 @@
           <t>تم التشغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>م.صيام</t>
@@ -4713,11 +4681,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4728,51 +4692,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>6\8\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4790,66 +4722,18 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4867,11 +4751,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4887,46 +4767,22 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>23\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4949,61 +4805,25 @@
           <t>641</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>15\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5026,11 +4846,7 @@
           <t>836</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5041,46 +4857,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>4\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -5098,66 +4886,18 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -5175,66 +4915,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -5252,66 +4944,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -5329,66 +4973,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -5406,66 +5002,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6223,47 +5771,123 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>21\7\2024</t>
@@ -6271,36 +5895,88 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6316,14 +5992,26 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>19\1\2025</t>
@@ -6331,29 +6019,61 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>573</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>573</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>8\4\2025</t>
@@ -6361,28 +6081,56 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>729</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>729</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6395,19 +6143,31 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>869</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>869</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6418,10 +6178,26 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>30\9\2025</t>
@@ -6429,84 +6205,252 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Event' to Card2 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,11 +529,6 @@
           <t>Correction</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Servised by</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -570,7 +565,6 @@
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -599,7 +593,6 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -628,7 +621,6 @@
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -657,7 +649,6 @@
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -710,7 +701,6 @@
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -755,7 +745,6 @@
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -784,7 +773,6 @@
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -813,7 +801,6 @@
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -842,7 +829,6 @@
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -871,7 +857,6 @@
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -900,7 +885,6 @@
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4535,7 +4519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4604,43 +4588,18 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Correction</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Servised by</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>150</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -4648,38 +4607,17 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1\2\2023</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>تم التشغيل</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>م.صيام</t>
-        </is>
-      </c>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>151</v>
+      </c>
+      <c r="C3" t="n">
+        <v>300</v>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
@@ -4702,25 +4640,16 @@
           <t>6\8\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>301</v>
+      </c>
+      <c r="C4" t="n">
+        <v>450</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -4731,25 +4660,16 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>451</v>
+      </c>
+      <c r="C5" t="n">
+        <v>550</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
@@ -4780,30 +4700,19 @@
           <t>23\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>641</t>
-        </is>
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>551</v>
+      </c>
+      <c r="C6" t="n">
+        <v>700</v>
+      </c>
+      <c r="D6" t="n">
+        <v>641</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -4821,30 +4730,19 @@
           <t>15\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>836</t>
-        </is>
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>701</v>
+      </c>
+      <c r="C7" t="n">
+        <v>850</v>
+      </c>
+      <c r="D7" t="n">
+        <v>836</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
@@ -4866,25 +4764,16 @@
           <t>4\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>851</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
@@ -4895,25 +4784,16 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1150</v>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
@@ -4924,25 +4804,16 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1151</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1300</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -4953,25 +4824,16 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1301</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1450</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -4982,25 +4844,16 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1451</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1500</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -5011,9 +4864,6 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5771,123 +5621,47 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>150</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>151</v>
+      </c>
+      <c r="C3" t="n">
+        <v>300</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>21\7\2024</t>
@@ -5895,88 +5669,36 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>301</v>
+      </c>
+      <c r="C4" t="n">
+        <v>450</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>451</v>
+      </c>
+      <c r="C5" t="n">
+        <v>550</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5992,26 +5714,14 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>19\1\2025</t>
@@ -6019,61 +5729,29 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>573</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>551</v>
+      </c>
+      <c r="C6" t="n">
+        <v>700</v>
+      </c>
+      <c r="D6" t="n">
+        <v>573</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>8\4\2025</t>
@@ -6081,56 +5759,28 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>729</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>701</v>
+      </c>
+      <c r="C7" t="n">
+        <v>850</v>
+      </c>
+      <c r="D7" t="n">
+        <v>729</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6143,31 +5793,19 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>869</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>851</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>869</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6178,26 +5816,10 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>30\9\2025</t>
@@ -6205,252 +5827,84 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1150</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1151</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1301</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1450</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1451</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8086,7 +7540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8155,38 +7609,96 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8197,28 +7709,59 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>16\7\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8234,89 +7777,210 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>27\2\2025</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>559</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>559</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>7\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>727</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>727</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8327,21 +7991,34 @@
           <t>6\7\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>860</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>860</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8352,125 +8029,347 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>28\9\2025</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>851</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D9" t="n">
-        <v>950</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>950</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L9" t="inlineStr">
         <is>
           <t>1\11\2025</t>
         </is>
       </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1450</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>2</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8483,7 +8382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8552,37 +8451,16 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Correction</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Servised by</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>150</v>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -8593,33 +8471,16 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>تم التشغيل</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>ا.نادر</t>
-        </is>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>151</v>
+      </c>
+      <c r="C3" t="n">
+        <v>300</v>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -8630,25 +8491,16 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>301</v>
+      </c>
+      <c r="C4" t="n">
+        <v>450</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -8659,25 +8511,16 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>451</v>
+      </c>
+      <c r="C5" t="n">
+        <v>550</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
@@ -8708,30 +8551,19 @@
           <t>25\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>629</t>
-        </is>
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>551</v>
+      </c>
+      <c r="C6" t="n">
+        <v>700</v>
+      </c>
+      <c r="D6" t="n">
+        <v>629</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -8749,30 +8581,19 @@
           <t>14\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>701</v>
+      </c>
+      <c r="C7" t="n">
+        <v>850</v>
+      </c>
+      <c r="D7" t="n">
+        <v>800</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
@@ -8794,25 +8615,16 @@
           <t>1\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>851</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
@@ -8823,25 +8635,16 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1150</v>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
@@ -8852,25 +8655,16 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1151</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1300</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -8881,25 +8675,16 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1301</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1450</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -8910,25 +8695,16 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1451</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1500</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -8939,9 +8715,6 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Correction' to Card2 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7540,7 +7540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7614,6 +7614,11 @@
           <t>Event</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -7676,7 +7681,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7739,7 +7749,12 @@
           <t>16\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7802,7 +7817,12 @@
           <t>27\2\2025</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7865,7 +7885,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7928,7 +7953,12 @@
           <t>7\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7991,7 +8021,12 @@
           <t>6\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8054,7 +8089,12 @@
           <t>28\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -8117,7 +8157,12 @@
           <t>1\11\2025</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8180,7 +8225,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8243,7 +8293,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8306,7 +8361,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -8369,7 +8429,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Servised by' to Card2 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7540,7 +7540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7619,6 +7619,11 @@
           <t>Correction</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Servised by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -7686,7 +7691,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7754,7 +7764,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7822,7 +7837,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7890,7 +7910,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7958,7 +7983,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8026,7 +8056,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8094,7 +8129,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -8162,7 +8202,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8230,7 +8275,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8298,7 +8348,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8366,7 +8421,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -8434,7 +8494,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Edit sheet Card18 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7540,7 +7540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7609,116 +7609,38 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Correction</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Servised by</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr"/>
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>150</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>151</v>
+      </c>
+      <c r="C3" t="n">
+        <v>300</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7729,69 +7651,28 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>16\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>301</v>
+      </c>
+      <c r="C4" t="n">
+        <v>450</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7807,240 +7688,89 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
           <t>27\2\2025</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr"/>
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>451</v>
+      </c>
+      <c r="C5" t="n">
+        <v>550</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>559</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>551</v>
+      </c>
+      <c r="C6" t="n">
+        <v>700</v>
+      </c>
+      <c r="D6" t="n">
+        <v>559</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>7\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>727</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>701</v>
+      </c>
+      <c r="C7" t="n">
+        <v>850</v>
+      </c>
+      <c r="D7" t="n">
+        <v>727</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8051,44 +7781,21 @@
           <t>6\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>860</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>851</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>860</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8099,407 +7806,125 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>28\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>950</t>
-        </is>
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
+        <v>851</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>950</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
           <t>1\11\2025</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr"/>
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1001</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1150</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr"/>
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1151</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr"/>
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1301</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1450</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr"/>
+      <c r="A13" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1451</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9943,47 +9368,123 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>1\12\2024</t>
@@ -9991,37 +9492,93 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10032,10 +9589,26 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>11\3\2025</t>
@@ -10043,21 +9616,41 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>590</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>590</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10068,8 +9661,16 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>29\4\2025</t>
@@ -10077,29 +9678,61 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>785</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>785</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>20\8\2025</t>
@@ -10107,19 +9740,31 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>883</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>883</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10130,10 +9775,26 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>23\10\2025</t>
@@ -10141,84 +9802,252 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Event' to Card18 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,11 +529,6 @@
           <t>Correction</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Servised by</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -553,64 +548,23 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>1\1\1111\</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -628,66 +582,17 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -705,66 +610,17 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -782,66 +638,17 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -864,11 +671,7 @@
           <t>632</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -889,36 +692,15 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -941,11 +723,7 @@
           <t>870</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -956,46 +734,17 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>6\10\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1013,66 +762,17 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1090,66 +790,17 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1167,66 +818,17 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1244,66 +846,17 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1321,66 +874,17 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9793,7 +9297,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9862,6 +9366,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -9879,15 +9388,52 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -9905,23 +9451,52 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>1\12\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -9939,15 +9514,52 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -9965,8 +9577,16 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -9977,15 +9597,32 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>11\3\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -10008,9 +9645,21 @@
           <t>590</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10021,13 +9670,22 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>29\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -10050,22 +9708,47 @@
           <t>785</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>20\8\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -10088,7 +9771,11 @@
           <t>883</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10099,15 +9786,32 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>23\10\2025</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -10125,15 +9829,52 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -10151,15 +9892,52 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -10177,15 +9955,52 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -10203,15 +10018,52 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Correction' to Card18 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -9297,7 +9297,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9371,6 +9371,11 @@
           <t>Event</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -9433,7 +9438,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -9496,7 +9506,12 @@
           <t>1\12\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -9559,7 +9574,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -9622,7 +9642,12 @@
           <t>11\3\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -9685,7 +9710,12 @@
           <t>29\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -9748,7 +9778,12 @@
           <t>20\8\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -9811,7 +9846,12 @@
           <t>23\10\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -9874,7 +9914,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -9937,7 +9982,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -10000,7 +10050,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -10063,7 +10118,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Servised by' to Card18 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -9297,7 +9297,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9376,6 +9376,11 @@
           <t>Correction</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Servised by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -9443,7 +9448,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -9511,7 +9521,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -9579,7 +9594,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -9647,7 +9667,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -9715,7 +9740,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -9783,7 +9813,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -9851,7 +9886,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -9919,7 +9959,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -9987,7 +10032,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -10055,7 +10105,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -10123,7 +10178,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Event ' to Card2 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -556,56 +556,20 @@
           <t>1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
           <t>1\1\1111\</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -624,61 +588,17 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -697,61 +617,17 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -770,61 +646,17 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -848,11 +680,7 @@
           <t>632</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -873,31 +701,15 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
@@ -921,11 +733,7 @@
           <t>870</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -936,41 +744,17 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>6\10\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -989,61 +773,17 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -1062,61 +802,17 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -1135,61 +831,17 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -1208,61 +860,17 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -1281,61 +889,17 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
@@ -7992,7 +7556,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8061,38 +7625,96 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Event </t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8103,28 +7725,59 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>16\7\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8140,89 +7793,210 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>27\2\2025</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>559</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>559</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>7\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>727</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>727</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8233,21 +8007,34 @@
           <t>6\7\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>860</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>860</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8258,125 +8045,347 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>28\9\2025</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>851</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D9" t="n">
-        <v>950</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>950</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L9" t="inlineStr">
         <is>
           <t>1\11\2025</t>
         </is>
       </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1450</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>2</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Correction ' to Card2 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7556,7 +7556,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7627,7 +7627,12 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Event </t>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Correction </t>
         </is>
       </c>
     </row>
@@ -7692,7 +7697,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7755,7 +7765,12 @@
           <t>16\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7818,7 +7833,12 @@
           <t>27\2\2025</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7881,7 +7901,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7944,7 +7969,12 @@
           <t>7\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8007,7 +8037,12 @@
           <t>6\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8070,7 +8105,12 @@
           <t>28\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -8133,7 +8173,12 @@
           <t>1\11\2025</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8196,7 +8241,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8259,7 +8309,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8322,7 +8377,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -8385,7 +8445,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Serviced by ' to Card2 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7556,7 +7556,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7632,7 +7632,12 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Correction </t>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serviced by </t>
         </is>
       </c>
     </row>
@@ -7702,7 +7707,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7770,7 +7780,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7838,7 +7853,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7906,7 +7926,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7974,7 +7999,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8042,7 +8072,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8110,7 +8145,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -8178,7 +8218,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8246,7 +8291,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8314,7 +8364,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8382,7 +8437,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -8450,7 +8510,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Edit sheet Card2 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -7637,7 +7637,7 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Serviced by </t>
+          <t>Serviced by</t>
         </is>
       </c>
     </row>
@@ -7712,7 +7712,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7785,7 +7789,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7858,7 +7866,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7931,7 +7943,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8004,7 +8020,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8077,7 +8097,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8150,7 +8174,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -8215,7 +8243,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">تم سن الفلاتس ومعايرته </t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -8223,7 +8251,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8296,7 +8328,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8369,7 +8405,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8442,7 +8482,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -8515,7 +8559,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>